<commit_message>
Data import and plotting
</commit_message>
<xml_diff>
--- a/data/220126Filled_site_info.xlsx
+++ b/data/220126Filled_site_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sydneywatercorporation-my.sharepoint.com/personal/2gt_sydneywater_com_au/Documents/Project/Berowra/_Data_Outgoing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Berowra\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F648EA2C-CD16-4CA9-9AA6-85E64A150264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F252AD6F-2F66-491F-BEB4-F662B20FA9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>Site Code</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Agency Code</t>
-  </si>
-  <si>
-    <t>NB11</t>
-  </si>
-  <si>
-    <t>NB13</t>
   </si>
   <si>
     <t>HSC</t>
@@ -890,12 +884,12 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>37</v>
       </c>
@@ -920,10 +914,10 @@
         <v>6288803.9763799999</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>41</v>
       </c>
@@ -934,10 +928,10 @@
         <v>6278229.8557099998</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>48</v>
       </c>
@@ -948,10 +942,10 @@
         <v>6289126.00648</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -962,10 +956,10 @@
         <v>6280725.6882100003</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>61</v>
       </c>
@@ -976,10 +970,10 @@
         <v>6282081.6645999998</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>67</v>
       </c>
@@ -990,10 +984,10 @@
         <v>6286141.1954800002</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>68</v>
       </c>
@@ -1004,10 +998,10 @@
         <v>6287056.0907800002</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>69</v>
       </c>
@@ -1018,10 +1012,10 @@
         <v>6288037.9693700001</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>90</v>
       </c>
@@ -1032,10 +1026,10 @@
         <v>6277423.0104200002</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>97</v>
       </c>
@@ -1046,10 +1040,10 @@
         <v>6279233.4805100001</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>100</v>
       </c>
@@ -1060,10 +1054,10 @@
         <v>6277790.4301199997</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>118</v>
       </c>
@@ -1074,10 +1068,10 @@
         <v>6277611.9992199996</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>151</v>
       </c>
@@ -1088,10 +1082,10 @@
         <v>6288209.97597</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>210</v>
       </c>
@@ -1102,12 +1096,12 @@
         <v>6285440.4602800002</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>11</v>
       </c>
       <c r="B16">
         <v>328096.60600000003</v>
@@ -1116,12 +1110,12 @@
         <v>6284349.3329999996</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>13</v>
       </c>
       <c r="B17">
         <v>325352.31300000002</v>
@@ -1130,10 +1124,10 @@
         <v>6282059.0839999998</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>

</xml_diff>